<commit_message>
refactor: update tutorial examples
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD71D7EB-166F-4FC5-8072-8DE5126CFE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A985ED1-7AE3-461A-A050-89B5F0ADF3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="116">
   <si>
     <t>role</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>default_view_version</t>
-  </si>
-  <si>
     <t>Definition of Containers</t>
   </si>
   <si>
@@ -388,7 +385,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,12 +438,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -511,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -539,12 +530,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -766,10 +756,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1001"/>
+  <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -796,10 +786,10 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
@@ -1041,12 +1031,8 @@
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -6270,29 +6256,7 @@
       <c r="W220" s="5"/>
     </row>
     <row r="221" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="5"/>
-      <c r="B221" s="4"/>
-      <c r="C221" s="5"/>
-      <c r="D221" s="5"/>
-      <c r="E221" s="5"/>
-      <c r="F221" s="5"/>
-      <c r="G221" s="5"/>
-      <c r="H221" s="5"/>
-      <c r="I221" s="5"/>
-      <c r="J221" s="5"/>
-      <c r="K221" s="5"/>
-      <c r="L221" s="5"/>
-      <c r="M221" s="5"/>
-      <c r="N221" s="5"/>
-      <c r="O221" s="5"/>
-      <c r="P221" s="5"/>
-      <c r="Q221" s="5"/>
-      <c r="R221" s="5"/>
-      <c r="S221" s="5"/>
-      <c r="T221" s="5"/>
-      <c r="U221" s="5"/>
-      <c r="V221" s="5"/>
-      <c r="W221" s="5"/>
+      <c r="B221" s="2"/>
     </row>
     <row r="222" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B222" s="2"/>
@@ -8630,9 +8594,6 @@
     </row>
     <row r="1000" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1000" s="2"/>
-    </row>
-    <row r="1001" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1001" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -8664,15 +8625,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="A1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -8693,26 +8654,26 @@
       <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>97</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -8724,10 +8685,10 @@
         <v>27</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -8741,7 +8702,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -8758,7 +8719,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -8772,7 +8733,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -8808,10 +8769,10 @@
     </row>
     <row r="9" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -8822,10 +8783,10 @@
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
@@ -8836,13 +8797,13 @@
     </row>
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -8889,10 +8850,10 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
         <v>49</v>
@@ -8903,10 +8864,10 @@
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>49</v>
@@ -8917,10 +8878,10 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -8928,10 +8889,10 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -8939,13 +8900,13 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -8953,10 +8914,10 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -8970,7 +8931,7 @@
         <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -8984,7 +8945,7 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -8998,7 +8959,7 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -10040,7 +10001,7 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
@@ -10072,72 +10033,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="A1" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="Q2" s="6"/>
@@ -10149,42 +10110,42 @@
       <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="17" t="b">
+      <c r="G3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="17" t="b">
+      <c r="H3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="17"/>
+      <c r="P3" s="16"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
@@ -10193,40 +10154,40 @@
       <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="17" t="b">
+      <c r="G4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="17" t="b">
+      <c r="H4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -10234,2327 +10195,2327 @@
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="17" t="b">
+      <c r="G5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="17" t="b">
+      <c r="H5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17" t="s">
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="17" t="b">
+      <c r="G6" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="17" t="b">
+      <c r="H6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="18" t="b">
+      <c r="G8" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="18" t="b">
+      <c r="H8" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="18" t="b">
+      <c r="G9" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="18" t="b">
+      <c r="H9" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="18" t="b">
+      <c r="G10" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="18" t="b">
+      <c r="H10" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="18" t="b">
+      <c r="G11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="18" t="b">
+      <c r="H11" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18" t="s">
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="18" t="b">
+      <c r="G12" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="18" t="b">
+      <c r="H12" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18" t="s">
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
     </row>
     <row r="13" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="14" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="17" t="b">
+      <c r="G14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="17" t="b">
+      <c r="H14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17" t="s">
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="17" t="b">
+      <c r="G15" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="17" t="b">
+      <c r="H15" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17" t="s">
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="17" t="s">
+      <c r="N15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="17" t="b">
+      <c r="G16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="17" t="b">
+      <c r="H16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="17" t="s">
+      <c r="M16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N16" s="17" t="s">
+      <c r="N16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
     </row>
     <row r="17" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="17" t="b">
+      <c r="G17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H17" s="17" t="b">
+      <c r="H17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17" t="s">
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="L17" s="17" t="s">
+      <c r="L17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="18" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18" t="b">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="18" t="s">
+      <c r="N19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
     </row>
     <row r="20" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="18" t="b">
+      <c r="G20" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H20" s="18" t="b">
+      <c r="H20" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18" t="s">
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="N20" s="18" t="s">
+      <c r="N20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18" t="b">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18" t="s">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="N21" s="18" t="s">
+      <c r="N21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="18" t="b">
+      <c r="G22" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H22" s="18" t="b">
+      <c r="H22" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18" t="s">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="18" t="s">
+      <c r="L22" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="N22" s="18" t="s">
+      <c r="N22" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="17" t="b">
+      <c r="G24" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="17" t="b">
+      <c r="H24" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17" t="s">
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="L24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="17" t="s">
+      <c r="N24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="17" t="b">
+      <c r="G25" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="17" t="b">
+      <c r="H25" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17" t="s">
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="17" t="s">
+      <c r="L25" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="17" t="s">
+      <c r="M25" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N25" s="17" t="s">
+      <c r="N25" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="17" t="b">
+      <c r="G26" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="H26" s="17" t="b">
+      <c r="H26" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17" t="s">
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="17" t="s">
+      <c r="L26" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="M26" s="17" t="s">
+      <c r="M26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N26" s="17" t="s">
+      <c r="N26" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="17" t="b">
+      <c r="G27" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="17" t="b">
+      <c r="H27" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17" t="s">
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="17" t="s">
+      <c r="L27" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="17" t="s">
+      <c r="M27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N27" s="17" t="s">
+      <c r="N27" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="18" t="b">
+      <c r="G29" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H29" s="18" t="b">
+      <c r="H29" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18" t="s">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L29" s="18" t="s">
+      <c r="L29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M29" s="18" t="s">
+      <c r="M29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="18" t="s">
+      <c r="N29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18" t="s">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="18" t="b">
+      <c r="G30" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H30" s="18" t="b">
+      <c r="H30" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18" t="s">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="18" t="s">
+      <c r="L30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M30" s="18" t="s">
+      <c r="M30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N30" s="18" t="s">
+      <c r="N30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" s="18" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18" t="b">
+      <c r="G31" s="17"/>
+      <c r="H31" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18" t="s">
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N31" s="18" t="s">
+      <c r="N31" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="18" t="s">
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18" t="b">
+      <c r="G32" s="17"/>
+      <c r="H32" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18" t="s">
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N32" s="18" t="s">
+      <c r="N32" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="18" t="s">
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18" t="b">
+      <c r="G33" s="17"/>
+      <c r="H33" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18" t="s">
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N33" s="18" t="s">
+      <c r="N33" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18" t="s">
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="18" t="b">
+      <c r="G34" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H34" s="18" t="b">
+      <c r="H34" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18" t="s">
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L34" s="18" t="s">
+      <c r="L34" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="M34" s="18" t="s">
+      <c r="M34" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="18" t="s">
+      <c r="N34" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18" t="s">
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G35" s="18" t="b">
+      <c r="G35" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H35" s="18" t="b">
+      <c r="H35" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18" t="s">
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L35" s="18" t="s">
+      <c r="L35" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M35" s="18" t="s">
+      <c r="M35" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N35" s="18" t="s">
+      <c r="N35" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
       <c r="R35" s="8"/>
       <c r="S35" s="9"/>
       <c r="T35" s="8"/>
       <c r="U35" s="8"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18" t="s">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="18" t="b">
+      <c r="G36" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H36" s="18" t="b">
+      <c r="H36" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18" t="s">
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L36" s="18" t="s">
+      <c r="L36" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="M36" s="18" t="s">
+      <c r="M36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N36" s="18" t="s">
+      <c r="N36" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
       <c r="R36" s="8"/>
       <c r="S36" s="9"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18" t="s">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="18" t="b">
+      <c r="G37" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H37" s="18" t="b">
+      <c r="H37" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18" t="s">
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="18" t="s">
+      <c r="L37" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="M37" s="18" t="s">
+      <c r="M37" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N37" s="18" t="s">
+      <c r="N37" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
       <c r="R37" s="8"/>
       <c r="S37" s="9"/>
       <c r="T37" s="8"/>
       <c r="U37" s="8"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18" t="s">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="18" t="b">
+      <c r="G38" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H38" s="18" t="b">
+      <c r="H38" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18" t="s">
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="18" t="s">
+      <c r="L38" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="M38" s="18" t="s">
+      <c r="M38" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N38" s="18" t="s">
+      <c r="N38" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
       <c r="R38" s="8"/>
       <c r="S38" s="9"/>
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
       <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" s="17" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17" t="b">
+      <c r="G40" s="16"/>
+      <c r="H40" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17" t="s">
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N40" s="17" t="s">
+      <c r="N40" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17" t="s">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="17" t="b">
+      <c r="G41" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H41" s="17" t="b">
+      <c r="H41" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17" t="s">
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="L41" s="17" t="s">
+      <c r="L41" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="M41" s="17" t="s">
+      <c r="M41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N41" s="17" t="s">
+      <c r="N41" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+    </row>
+    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="N46" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+    </row>
+    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="N47" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+    </row>
+    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18" t="s">
+      <c r="B49" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" s="18" t="b">
+      <c r="F49" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H43" s="18" t="b">
+      <c r="H49" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18" t="s">
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="L43" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M43" s="18" t="s">
+      <c r="L49" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="M49" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="N43" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-    </row>
-    <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+      <c r="N49" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18" t="s">
+      <c r="B50" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="N50" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="L51" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="M51" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="N51" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+    </row>
+    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+    </row>
+    <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="L53" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="N53" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+    </row>
+    <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44" s="18" t="b">
+      <c r="F54" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G54" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H44" s="18" t="b">
+      <c r="H54" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="L44" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="M44" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="N44" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-    </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-    </row>
-    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17" t="s">
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="L54" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M54" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M55" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="N57" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M59" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+    </row>
+    <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="M60" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+    </row>
+    <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+    </row>
+    <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+    </row>
+    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N64" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+    </row>
+    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+    </row>
+    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="L66" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="M66" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+    </row>
+    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+    </row>
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G46" s="17" t="b">
+      <c r="F68" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H46" s="17" t="b">
+      <c r="H68" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-    </row>
-    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17" t="b">
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="L68" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M68" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N68" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G69" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="N47" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-    </row>
-    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-    </row>
-    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G49" s="18" t="b">
+      <c r="H69" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="L69" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M69" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N69" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="O69" s="16"/>
+      <c r="P69" s="16"/>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+    </row>
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="L71" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M71" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+      <c r="J72" s="17"/>
+      <c r="K72" s="17"/>
+      <c r="L72" s="17"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+    </row>
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="H49" s="18" t="b">
+      <c r="H73" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="L49" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="M49" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="N49" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18" t="b">
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L73" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="M73" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="N73" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+    </row>
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="16"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+    </row>
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="N50" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-    </row>
-    <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G51" s="18" t="b">
+      <c r="H75" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H51" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="L51" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="M51" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="N51" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-    </row>
-    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-    </row>
-    <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H53" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L53" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="N53" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O53" s="17"/>
-      <c r="P53" s="17"/>
-    </row>
-    <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H54" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L54" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-    </row>
-    <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G55" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L55" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="M55" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
-    </row>
-    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-    </row>
-    <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G57" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="L57" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="M57" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="N57" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-    </row>
-    <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
-    </row>
-    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H59" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L59" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="M59" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="N59" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
-    </row>
-    <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-      <c r="K60" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L60" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="M60" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="N60" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="O60" s="17"/>
-      <c r="P60" s="17"/>
-    </row>
-    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
-    </row>
-    <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="N62" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-    </row>
-    <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-    </row>
-    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I64" s="17"/>
-      <c r="J64" s="17"/>
-      <c r="K64" s="17"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="N64" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
-    </row>
-    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="17"/>
-    </row>
-    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" s="18" t="s">
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L75" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G66" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="L66" s="18" t="s">
+      <c r="M75" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N75" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="M66" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="N66" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="O66" s="18"/>
-      <c r="P66" s="18"/>
-    </row>
-    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="18"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="18"/>
-    </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G68" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H68" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-      <c r="K68" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="L68" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="M68" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
-    </row>
-    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G69" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H69" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="L69" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="M69" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="N69" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-    </row>
-    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-    </row>
-    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="L71" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="M71" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="N71" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="O71" s="18"/>
-      <c r="P71" s="18"/>
-    </row>
-    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-      <c r="L72" s="18"/>
-      <c r="M72" s="18"/>
-      <c r="N72" s="18"/>
-      <c r="O72" s="18"/>
-      <c r="P72" s="18"/>
-    </row>
-    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G73" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H73" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="L73" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="M73" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="N73" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-    </row>
-    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
-    </row>
-    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G75" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H75" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="L75" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="M75" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="N75" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="O75" s="18"/>
-      <c r="P75" s="18"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
     </row>
     <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="10"/>
@@ -24743,13 +24704,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="A1" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -24771,19 +24732,19 @@
       <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="6"/>
@@ -24854,13 +24815,13 @@
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -24869,10 +24830,10 @@
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -24885,26 +24846,26 @@
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -24915,7 +24876,7 @@
         <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
tests: upgrade test data
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAA10B7-5E78-4EF6-91B0-5917F6763ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18333C5E-87E1-4823-AFE5-F0A086B6FDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Container</t>
-  </si>
-  <si>
-    <t>ContainerProperty</t>
   </si>
   <si>
     <t>View</t>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>In Model</t>
+  </si>
+  <si>
+    <t>Container Property</t>
   </si>
 </sst>
 </file>
@@ -786,18 +786,18 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -831,10 +831,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="5"/>
@@ -887,10 +887,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -919,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -945,10 +945,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="12">
         <v>45351.489040733439</v>
@@ -8608,8 +8608,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8641,7 +8641,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -8661,19 +8661,19 @@
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -8682,31 +8682,31 @@
         <v>8</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="M2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="O2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -8718,16 +8718,16 @@
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="16" t="b">
         <v>0</v>
@@ -8738,20 +8738,20 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="16"/>
       <c r="O3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -8762,16 +8762,16 @@
     </row>
     <row r="4" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="16" t="b">
         <v>0</v>
@@ -8782,18 +8782,18 @@
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
@@ -8803,20 +8803,20 @@
     </row>
     <row r="5" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>106</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="16" t="b">
         <v>0</v>
@@ -8827,18 +8827,18 @@
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>23</v>
       </c>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>23</v>
       </c>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
@@ -8847,18 +8847,18 @@
     </row>
     <row r="6" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="16" t="b">
         <v>1</v>
@@ -8868,21 +8868,21 @@
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
@@ -8913,16 +8913,16 @@
     </row>
     <row r="8" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="17" t="b">
         <v>1</v>
@@ -8933,18 +8933,18 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
@@ -8953,16 +8953,16 @@
     </row>
     <row r="9" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="17" t="b">
         <v>0</v>
@@ -8973,32 +8973,32 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="17" t="b">
         <v>0</v>
@@ -9009,18 +9009,18 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
@@ -9029,18 +9029,18 @@
     </row>
     <row r="11" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" s="17" t="b">
         <v>1</v>
@@ -9051,18 +9051,18 @@
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
@@ -9071,16 +9071,16 @@
     </row>
     <row r="12" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="17" t="b">
         <v>1</v>
@@ -9091,18 +9091,18 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
@@ -9125,16 +9125,16 @@
     </row>
     <row r="14" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="16" t="b">
         <v>0</v>
@@ -9145,18 +9145,18 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
@@ -9165,18 +9165,18 @@
     </row>
     <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" s="16" t="b">
         <v>1</v>
@@ -9187,18 +9187,18 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
@@ -9207,16 +9207,16 @@
     </row>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="16" t="b">
         <v>0</v>
@@ -9227,18 +9227,18 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
@@ -9247,16 +9247,16 @@
     </row>
     <row r="17" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="16" t="b">
         <v>0</v>
@@ -9267,18 +9267,18 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
@@ -9309,18 +9309,18 @@
     </row>
     <row r="19" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17" t="b">
@@ -9333,26 +9333,26 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="17" t="b">
         <v>1</v>
@@ -9363,18 +9363,18 @@
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
@@ -9383,18 +9383,18 @@
     </row>
     <row r="21" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17" t="b">
@@ -9407,10 +9407,10 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
@@ -9419,18 +9419,18 @@
     </row>
     <row r="22" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G22" s="17" t="b">
         <v>1</v>
@@ -9441,18 +9441,18 @@
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
@@ -9477,18 +9477,18 @@
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="16" t="b">
         <v>1</v>
@@ -9499,18 +9499,18 @@
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P24" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
@@ -9519,18 +9519,18 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G25" s="16" t="b">
         <v>1</v>
@@ -9541,18 +9541,18 @@
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P25" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
@@ -9561,16 +9561,16 @@
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="16" t="b">
         <v>0</v>
@@ -9581,32 +9581,32 @@
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27" s="16" t="b">
         <v>1</v>
@@ -9617,18 +9617,18 @@
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P27" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
@@ -9659,16 +9659,16 @@
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="17" t="b">
         <v>0</v>
@@ -9679,18 +9679,18 @@
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
       <c r="O29" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P29" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
@@ -9699,16 +9699,16 @@
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" s="17" t="b">
         <v>1</v>
@@ -9719,18 +9719,18 @@
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
@@ -9739,18 +9739,18 @@
     </row>
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="b">
@@ -9763,10 +9763,10 @@
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
       <c r="O31" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
@@ -9775,18 +9775,18 @@
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17" t="b">
@@ -9799,10 +9799,10 @@
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
       <c r="O32" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
@@ -9811,18 +9811,18 @@
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17" t="b">
@@ -9835,10 +9835,10 @@
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
       <c r="O33" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P33" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
@@ -9847,18 +9847,18 @@
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G34" s="17" t="b">
         <v>1</v>
@@ -9869,34 +9869,34 @@
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P34" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G35" s="17" t="b">
         <v>1</v>
@@ -9907,18 +9907,18 @@
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P35" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R35" s="8"/>
       <c r="S35" s="9"/>
@@ -9927,18 +9927,18 @@
     </row>
     <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G36" s="17" t="b">
         <v>1</v>
@@ -9949,18 +9949,18 @@
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
       <c r="O36" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P36" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R36" s="8"/>
       <c r="S36" s="9"/>
@@ -9969,16 +9969,16 @@
     </row>
     <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G37" s="17" t="b">
         <v>0</v>
@@ -9989,18 +9989,18 @@
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
       <c r="O37" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P37" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R37" s="8"/>
       <c r="S37" s="9"/>
@@ -10009,16 +10009,16 @@
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G38" s="17" t="b">
         <v>0</v>
@@ -10029,18 +10029,18 @@
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P38" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R38" s="8"/>
       <c r="S38" s="9"/>
@@ -10068,18 +10068,18 @@
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="16" t="b">
@@ -10092,26 +10092,26 @@
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P40" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G41" s="16" t="b">
         <v>1</v>
@@ -10122,18 +10122,18 @@
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P41" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10156,18 +10156,18 @@
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" s="17" t="b">
         <v>1</v>
@@ -10178,34 +10178,34 @@
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
       <c r="O43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P43" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G44" s="17" t="b">
         <v>1</v>
@@ -10216,18 +10216,18 @@
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P44" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10250,18 +10250,18 @@
     </row>
     <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G46" s="16" t="b">
         <v>1</v>
@@ -10272,34 +10272,34 @@
       <c r="I46" s="16"/>
       <c r="J46" s="16"/>
       <c r="K46" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P46" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16" t="b">
@@ -10312,10 +10312,10 @@
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
       <c r="O47" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10338,18 +10338,18 @@
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="17" t="b">
         <v>1</v>
@@ -10360,34 +10360,34 @@
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P49" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17" t="b">
@@ -10400,24 +10400,24 @@
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P50" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
       <c r="F51" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G51" s="17" t="b">
         <v>0</v>
@@ -10428,18 +10428,18 @@
       <c r="I51" s="17"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L51" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P51" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10462,16 +10462,16 @@
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G53" s="16" t="b">
         <v>0</v>
@@ -10482,34 +10482,34 @@
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L53" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P53" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G54" s="16" t="b">
         <v>1</v>
@@ -10520,32 +10520,32 @@
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P54" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G55" s="16" t="b">
         <v>0</v>
@@ -10556,18 +10556,18 @@
       <c r="I55" s="16"/>
       <c r="J55" s="16"/>
       <c r="K55" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L55" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
       <c r="O55" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P55" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10590,16 +10590,16 @@
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G57" s="17" t="b">
         <v>0</v>
@@ -10610,18 +10610,18 @@
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
       <c r="K57" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L57" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
       <c r="O57" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P57" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10644,16 +10644,16 @@
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="F59" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G59" s="16" t="b">
         <v>0</v>
@@ -10664,32 +10664,32 @@
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L59" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P59" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G60" s="16" t="b">
         <v>0</v>
@@ -10700,18 +10700,18 @@
       <c r="I60" s="16"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
       <c r="O60" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P60" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10734,18 +10734,18 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17" t="b">
@@ -10758,10 +10758,10 @@
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
       <c r="O62" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P62" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10784,18 +10784,18 @@
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
       <c r="E64" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16" t="b">
@@ -10808,10 +10808,10 @@
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P64" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10834,16 +10834,16 @@
     </row>
     <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G66" s="17" t="b">
         <v>1</v>
@@ -10854,18 +10854,18 @@
       <c r="I66" s="17"/>
       <c r="J66" s="17"/>
       <c r="K66" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L66" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="L66" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="M66" s="17"/>
       <c r="N66" s="17"/>
       <c r="O66" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="P66" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="P66" s="17" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10888,18 +10888,18 @@
     </row>
     <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G68" s="16" t="b">
         <v>1</v>
@@ -10910,34 +10910,34 @@
       <c r="I68" s="16"/>
       <c r="J68" s="16"/>
       <c r="K68" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L68" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="L68" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
       <c r="O68" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P68" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="P68" s="16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G69" s="16" t="b">
         <v>1</v>
@@ -10948,18 +10948,18 @@
       <c r="I69" s="16"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L69" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P69" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10982,16 +10982,16 @@
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G71" s="17" t="b">
         <v>0</v>
@@ -11002,18 +11002,18 @@
       <c r="I71" s="17"/>
       <c r="J71" s="17"/>
       <c r="K71" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="L71" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="L71" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="P71" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="P71" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11036,16 +11036,16 @@
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G73" s="16" t="b">
         <v>1</v>
@@ -11056,18 +11056,18 @@
       <c r="I73" s="16"/>
       <c r="J73" s="16"/>
       <c r="K73" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L73" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M73" s="16"/>
       <c r="N73" s="16"/>
       <c r="O73" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P73" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11090,16 +11090,16 @@
     </row>
     <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G75" s="17" t="b">
         <v>1</v>
@@ -11110,18 +11110,18 @@
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
       <c r="K75" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L75" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M75" s="17"/>
       <c r="N75" s="17"/>
       <c r="O75" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P75" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -23295,7 +23295,7 @@
   </sheetPr>
   <dimension ref="A1:Y993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -23312,7 +23312,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -23341,369 +23341,369 @@
     </row>
     <row r="2" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -24703,7 +24703,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -24734,187 +24734,187 @@
         <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: min-max count alice rules
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5939716-1841-4D0F-80E7-BB04D4A5982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860A2AE6-1D6F-4793-A5A4-19CB8F9520FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Value Type</t>
-  </si>
-  <si>
-    <t>Nullable</t>
   </si>
   <si>
     <t>Default</t>
@@ -363,9 +360,6 @@
     <t>Connection</t>
   </si>
   <si>
-    <t>Is List</t>
-  </si>
-  <si>
     <t>Class (linage)</t>
   </si>
   <si>
@@ -379,6 +373,12 @@
   </si>
   <si>
     <t>Immutable</t>
+  </si>
+  <si>
+    <t>Max Count</t>
+  </si>
+  <si>
+    <t>Min Count</t>
   </si>
 </sst>
 </file>
@@ -789,18 +789,18 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -834,10 +834,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -863,7 +863,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="5"/>
@@ -890,10 +890,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -922,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -948,10 +948,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -977,7 +977,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="12">
         <v>45351.489040733439</v>
@@ -8612,7 +8612,7 @@
   <dimension ref="A1:X1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8644,7 +8644,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="78" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -8665,55 +8665,55 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="15" t="s">
+      <c r="K2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -8725,43 +8725,43 @@
     </row>
     <row r="3" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1</v>
       </c>
       <c r="H3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="16" t="b">
-        <v>0</v>
+      <c r="I3" s="16">
+        <v>1</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
@@ -8772,41 +8772,41 @@
     </row>
     <row r="4" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
       </c>
       <c r="H4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="16" t="b">
-        <v>0</v>
+      <c r="I4" s="16">
+        <v>1</v>
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -8816,45 +8816,45 @@
     </row>
     <row r="5" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>104</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>105</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
       </c>
       <c r="H5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="16" t="b">
-        <v>0</v>
+      <c r="I5" s="16">
+        <v>1</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
@@ -8863,45 +8863,45 @@
     </row>
     <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="16" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
       </c>
       <c r="H6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="16" t="b">
-        <v>0</v>
+      <c r="I6" s="16">
+        <v>1</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
@@ -8933,41 +8933,41 @@
     </row>
     <row r="8" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="17" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0</v>
       </c>
       <c r="H8" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="17" t="b">
-        <v>0</v>
+      <c r="I8" s="17">
+        <v>1</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -8976,80 +8976,80 @@
     </row>
     <row r="9" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
       </c>
       <c r="H9" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="17" t="b">
-        <v>0</v>
+      <c r="I9" s="17">
+        <v>1</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
       </c>
       <c r="H10" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="17" t="b">
-        <v>0</v>
+      <c r="I10" s="17">
+        <v>1</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
@@ -9058,43 +9058,43 @@
     </row>
     <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="17" t="b">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
       </c>
       <c r="H11" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="17" t="b">
-        <v>0</v>
+      <c r="I11" s="17">
+        <v>1</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
@@ -9103,41 +9103,41 @@
     </row>
     <row r="12" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="17" t="b">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
       </c>
       <c r="H12" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="17" t="b">
-        <v>0</v>
+      <c r="I12" s="17">
+        <v>1</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
@@ -9161,41 +9161,41 @@
     </row>
     <row r="14" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
       </c>
       <c r="H14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="16" t="b">
-        <v>0</v>
+      <c r="I14" s="16">
+        <v>1</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
       <c r="P14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
@@ -9204,43 +9204,43 @@
     </row>
     <row r="15" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="16" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
       </c>
       <c r="H15" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="16" t="b">
-        <v>0</v>
+      <c r="I15" s="16">
+        <v>1</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
@@ -9249,41 +9249,41 @@
     </row>
     <row r="16" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
       </c>
       <c r="H16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="16" t="b">
-        <v>0</v>
+      <c r="I16" s="16">
+        <v>1</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
       <c r="P16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
@@ -9292,41 +9292,41 @@
     </row>
     <row r="17" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1</v>
       </c>
       <c r="H17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="16" t="b">
-        <v>0</v>
+      <c r="I17" s="16">
+        <v>1</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
@@ -9358,24 +9358,22 @@
     </row>
     <row r="19" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
@@ -9383,51 +9381,51 @@
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="17" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0</v>
       </c>
       <c r="H20" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="17" t="b">
-        <v>0</v>
+      <c r="I20" s="17">
+        <v>1</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
@@ -9436,24 +9434,22 @@
     </row>
     <row r="21" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I21" s="17"/>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
@@ -9461,10 +9457,10 @@
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q21" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
@@ -9473,43 +9469,43 @@
     </row>
     <row r="22" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="17" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0</v>
       </c>
       <c r="H22" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="17" t="b">
-        <v>0</v>
+      <c r="I22" s="17">
+        <v>1</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
@@ -9535,43 +9531,43 @@
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
       </c>
       <c r="H24" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="16" t="b">
-        <v>0</v>
+      <c r="I24" s="16">
+        <v>1</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
@@ -9580,43 +9576,43 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="16" t="b">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
       </c>
       <c r="H25" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="16" t="b">
-        <v>0</v>
+      <c r="I25" s="16">
+        <v>1</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
       <c r="P25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
@@ -9625,80 +9621,80 @@
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
       </c>
       <c r="H26" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="16" t="b">
-        <v>0</v>
+      <c r="I26" s="16">
+        <v>1</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="16" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
       </c>
       <c r="H27" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="16" t="b">
-        <v>0</v>
+      <c r="I27" s="16">
+        <v>1</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
@@ -9730,41 +9726,41 @@
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="17" t="b">
+        <v>15</v>
+      </c>
+      <c r="G29" s="17">
         <v>0</v>
       </c>
       <c r="H29" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="17" t="b">
-        <v>0</v>
+      <c r="I29" s="17">
+        <v>1</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
@@ -9773,41 +9769,41 @@
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="17" t="b">
+        <v>15</v>
+      </c>
+      <c r="G30" s="17">
         <v>1</v>
       </c>
       <c r="H30" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="17" t="b">
-        <v>0</v>
+      <c r="I30" s="17">
+        <v>1</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
       <c r="L30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
@@ -9816,24 +9812,22 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
@@ -9841,10 +9835,10 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
@@ -9853,24 +9847,22 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I32" s="17"/>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
       <c r="L32" s="17"/>
@@ -9878,10 +9870,10 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q32" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
@@ -9890,24 +9882,22 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I33" s="17"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
       <c r="L33" s="17"/>
@@ -9915,10 +9905,10 @@
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
       <c r="P33" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
@@ -9927,84 +9917,84 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="17" t="b">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0</v>
       </c>
       <c r="H34" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="17" t="b">
-        <v>0</v>
+      <c r="I34" s="17">
+        <v>1</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N34" s="17"/>
       <c r="O34" s="17"/>
       <c r="P34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="17" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="G35" s="17">
+        <v>0</v>
       </c>
       <c r="H35" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="17" t="b">
-        <v>0</v>
+      <c r="I35" s="17">
+        <v>1</v>
       </c>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S35" s="8"/>
       <c r="T35" s="9"/>
@@ -10013,43 +10003,43 @@
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="17" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0</v>
       </c>
       <c r="H36" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="17" t="b">
-        <v>0</v>
+      <c r="I36" s="17">
+        <v>1</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N36" s="17"/>
       <c r="O36" s="17"/>
       <c r="P36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S36" s="8"/>
       <c r="T36" s="9"/>
@@ -10058,41 +10048,41 @@
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1</v>
       </c>
       <c r="H37" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="17" t="b">
-        <v>0</v>
+      <c r="I37" s="17">
+        <v>1</v>
       </c>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
       <c r="P37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S37" s="8"/>
       <c r="T37" s="9"/>
@@ -10101,41 +10091,41 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G38" s="17">
+        <v>1</v>
       </c>
       <c r="H38" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="17" t="b">
-        <v>0</v>
+      <c r="I38" s="17">
+        <v>1</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S38" s="8"/>
       <c r="T38" s="9"/>
@@ -10164,24 +10154,22 @@
     </row>
     <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
-      <c r="I40" s="16" t="b">
-        <v>1</v>
-      </c>
+      <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
@@ -10189,51 +10177,51 @@
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q40" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="16" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G41" s="16">
+        <v>0</v>
       </c>
       <c r="H41" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="16" t="b">
-        <v>0</v>
+      <c r="I41" s="16">
+        <v>1</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
       <c r="P41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10257,84 +10245,84 @@
     </row>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" s="17" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G43" s="17">
+        <v>0</v>
       </c>
       <c r="H43" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="17" t="b">
-        <v>0</v>
+      <c r="I43" s="17">
+        <v>1</v>
       </c>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
       <c r="P43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="17" t="b">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="G44" s="17">
+        <v>0</v>
       </c>
       <c r="H44" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="17" t="b">
-        <v>0</v>
+      <c r="I44" s="17">
+        <v>1</v>
       </c>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
       <c r="L44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N44" s="17"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10358,65 +10346,63 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="16" t="b">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="G46" s="16">
+        <v>0</v>
       </c>
       <c r="H46" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="16" t="b">
-        <v>0</v>
+      <c r="I46" s="16">
+        <v>1</v>
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
       <c r="L46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
       <c r="P46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="16" t="b">
-        <v>1</v>
-      </c>
+      <c r="I47" s="16"/>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>
       <c r="L47" s="16"/>
@@ -10424,10 +10410,10 @@
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
       <c r="P47" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10451,65 +10437,63 @@
     </row>
     <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" s="17" t="b">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="G49" s="17">
+        <v>0</v>
       </c>
       <c r="H49" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="17" t="b">
-        <v>0</v>
+      <c r="I49" s="17">
+        <v>1</v>
       </c>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
-      <c r="I50" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I50" s="17"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
@@ -10517,49 +10501,49 @@
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
       <c r="P50" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q50" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
       <c r="F51" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G51" s="17">
+        <v>1</v>
       </c>
       <c r="H51" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="17" t="b">
-        <v>0</v>
+      <c r="I51" s="17">
+        <v>1</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10583,121 +10567,121 @@
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="16" t="b">
+        <v>15</v>
+      </c>
+      <c r="G53" s="16">
         <v>0</v>
       </c>
       <c r="H53" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="16" t="b">
-        <v>0</v>
+      <c r="I53" s="16">
+        <v>1</v>
       </c>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
       <c r="L53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
       <c r="P53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G54" s="16" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="G54" s="16">
+        <v>0</v>
       </c>
       <c r="H54" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="16" t="b">
-        <v>0</v>
+      <c r="I54" s="16">
+        <v>1</v>
       </c>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
       <c r="L54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
       <c r="P54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G55" s="16">
+        <v>1</v>
       </c>
       <c r="H55" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I55" s="16" t="b">
-        <v>0</v>
+      <c r="I55" s="16">
+        <v>1</v>
       </c>
       <c r="J55" s="16"/>
       <c r="K55" s="16"/>
       <c r="L55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N55" s="16"/>
       <c r="O55" s="16"/>
       <c r="P55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10721,41 +10705,41 @@
     </row>
     <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="17" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G57" s="17">
+        <v>1</v>
       </c>
       <c r="H57" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="17" t="b">
-        <v>0</v>
+      <c r="I57" s="17">
+        <v>1</v>
       </c>
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
       <c r="L57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N57" s="17"/>
       <c r="O57" s="17"/>
       <c r="P57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10779,80 +10763,80 @@
     </row>
     <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="F59" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G59" s="16">
+        <v>1</v>
       </c>
       <c r="H59" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I59" s="16" t="b">
-        <v>0</v>
+      <c r="I59" s="16">
+        <v>1</v>
       </c>
       <c r="J59" s="16"/>
       <c r="K59" s="16"/>
       <c r="L59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
       <c r="P59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G60" s="16">
+        <v>1</v>
       </c>
       <c r="H60" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I60" s="16" t="b">
-        <v>0</v>
+      <c r="I60" s="16">
+        <v>1</v>
       </c>
       <c r="J60" s="16"/>
       <c r="K60" s="16"/>
       <c r="L60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N60" s="16"/>
       <c r="O60" s="16"/>
       <c r="P60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10876,24 +10860,22 @@
     </row>
     <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
-      <c r="I62" s="17" t="b">
-        <v>1</v>
-      </c>
+      <c r="I62" s="17"/>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
@@ -10901,10 +10883,10 @@
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
       <c r="P62" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q62" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10928,24 +10910,22 @@
     </row>
     <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
       <c r="E64" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="16" t="b">
-        <v>1</v>
-      </c>
+      <c r="I64" s="16"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
@@ -10953,10 +10933,10 @@
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
       <c r="P64" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q64" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10980,41 +10960,41 @@
     </row>
     <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" s="17" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G66" s="17">
+        <v>0</v>
       </c>
       <c r="H66" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I66" s="17" t="b">
-        <v>0</v>
+      <c r="I66" s="17">
+        <v>1</v>
       </c>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
       <c r="L66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="M66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="M66" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="N66" s="17"/>
       <c r="O66" s="17"/>
       <c r="P66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="Q66" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11038,84 +11018,84 @@
     </row>
     <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G68" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G68" s="16">
+        <v>0</v>
       </c>
       <c r="H68" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I68" s="16" t="b">
-        <v>0</v>
+      <c r="I68" s="16">
+        <v>1</v>
       </c>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
       <c r="L68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="M68" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
       <c r="P68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="Q68" s="16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G69" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G69" s="16">
+        <v>0</v>
       </c>
       <c r="H69" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I69" s="16" t="b">
-        <v>0</v>
+      <c r="I69" s="16">
+        <v>1</v>
       </c>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
       <c r="L69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
       <c r="P69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11139,41 +11119,41 @@
     </row>
     <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G71" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G71" s="17">
+        <v>1</v>
       </c>
       <c r="H71" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I71" s="17" t="b">
-        <v>0</v>
+      <c r="I71" s="17">
+        <v>1</v>
       </c>
       <c r="J71" s="17"/>
       <c r="K71" s="17"/>
       <c r="L71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="M71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="M71" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="N71" s="17"/>
       <c r="O71" s="17"/>
       <c r="P71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="Q71" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11197,41 +11177,41 @@
     </row>
     <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="16" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G73" s="16">
+        <v>0</v>
       </c>
       <c r="H73" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I73" s="16" t="b">
-        <v>0</v>
+      <c r="I73" s="16">
+        <v>1</v>
       </c>
       <c r="J73" s="16"/>
       <c r="K73" s="16"/>
       <c r="L73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N73" s="16"/>
       <c r="O73" s="16"/>
       <c r="P73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11255,41 +11235,41 @@
     </row>
     <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G75" s="17" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G75" s="17">
+        <v>0</v>
       </c>
       <c r="H75" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="17" t="b">
-        <v>0</v>
+      <c r="I75" s="17">
+        <v>1</v>
       </c>
       <c r="J75" s="17"/>
       <c r="K75" s="17"/>
       <c r="L75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N75" s="17"/>
       <c r="O75" s="17"/>
       <c r="P75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -24415,7 +24395,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -24444,369 +24424,369 @@
     </row>
     <row r="2" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -25806,7 +25786,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -25834,190 +25814,190 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor; inf to alice
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860A2AE6-1D6F-4793-A5A4-19CB8F9520FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7B1F3C-265D-4D8D-9A85-37622C9614A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="118">
   <si>
     <t>role</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Min Count</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -8612,7 +8615,7 @@
   <dimension ref="A1:X1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9373,7 +9376,9 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="I19" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
@@ -9449,7 +9454,9 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="I21" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
@@ -9827,7 +9834,9 @@
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="I31" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
@@ -9862,7 +9871,9 @@
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
+      <c r="I32" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
       <c r="L32" s="17"/>
@@ -9897,7 +9908,9 @@
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="I33" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
       <c r="L33" s="17"/>
@@ -10169,7 +10182,9 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
+      <c r="I40" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
@@ -10402,7 +10417,9 @@
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
+      <c r="I47" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>
       <c r="L47" s="16"/>
@@ -10493,7 +10510,9 @@
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="I50" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
@@ -10875,7 +10894,9 @@
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="I62" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
@@ -10925,7 +10946,9 @@
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
+      <c r="I64" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>

</xml_diff>

<commit_message>
[NEAT-787] ➕ Introducing min/max for DMS sheet (#1029)
# Description

Please describe the change you have made.

## Bump

- [ ] Patch
- [x] Minor
- [ ] Skip

## Changelog
### Added

- Properties `Min Count` and `Max Count` to DMS sheet.

### Removed

- The properties `Is List` and `Nullable` are now deprecated in the DMS
sheet, and instead derived from the Min Count` and `Max Count`.
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5939716-1841-4D0F-80E7-BB04D4A5982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7B1F3C-265D-4D8D-9A85-37622C9614A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="118">
   <si>
     <t>role</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Value Type</t>
-  </si>
-  <si>
-    <t>Nullable</t>
   </si>
   <si>
     <t>Default</t>
@@ -363,9 +360,6 @@
     <t>Connection</t>
   </si>
   <si>
-    <t>Is List</t>
-  </si>
-  <si>
     <t>Class (linage)</t>
   </si>
   <si>
@@ -379,6 +373,15 @@
   </si>
   <si>
     <t>Immutable</t>
+  </si>
+  <si>
+    <t>Max Count</t>
+  </si>
+  <si>
+    <t>Min Count</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -789,18 +792,18 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -834,10 +837,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -863,7 +866,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="5"/>
@@ -890,10 +893,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -922,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -948,10 +951,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -977,7 +980,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="12">
         <v>45351.489040733439</v>
@@ -8612,7 +8615,7 @@
   <dimension ref="A1:X1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8644,7 +8647,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="78" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -8665,55 +8668,55 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="15" t="s">
+      <c r="K2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -8725,43 +8728,43 @@
     </row>
     <row r="3" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1</v>
       </c>
       <c r="H3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="16" t="b">
-        <v>0</v>
+      <c r="I3" s="16">
+        <v>1</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
@@ -8772,41 +8775,41 @@
     </row>
     <row r="4" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
       </c>
       <c r="H4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="16" t="b">
-        <v>0</v>
+      <c r="I4" s="16">
+        <v>1</v>
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -8816,45 +8819,45 @@
     </row>
     <row r="5" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>104</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>105</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
       </c>
       <c r="H5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="16" t="b">
-        <v>0</v>
+      <c r="I5" s="16">
+        <v>1</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
@@ -8863,45 +8866,45 @@
     </row>
     <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="16" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
       </c>
       <c r="H6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="16" t="b">
-        <v>0</v>
+      <c r="I6" s="16">
+        <v>1</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
@@ -8933,41 +8936,41 @@
     </row>
     <row r="8" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="17" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0</v>
       </c>
       <c r="H8" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="17" t="b">
-        <v>0</v>
+      <c r="I8" s="17">
+        <v>1</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -8976,80 +8979,80 @@
     </row>
     <row r="9" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
       </c>
       <c r="H9" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="17" t="b">
-        <v>0</v>
+      <c r="I9" s="17">
+        <v>1</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
       </c>
       <c r="H10" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="17" t="b">
-        <v>0</v>
+      <c r="I10" s="17">
+        <v>1</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
@@ -9058,43 +9061,43 @@
     </row>
     <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="17" t="b">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
       </c>
       <c r="H11" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="17" t="b">
-        <v>0</v>
+      <c r="I11" s="17">
+        <v>1</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
@@ -9103,41 +9106,41 @@
     </row>
     <row r="12" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="17" t="b">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
       </c>
       <c r="H12" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="17" t="b">
-        <v>0</v>
+      <c r="I12" s="17">
+        <v>1</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
@@ -9161,41 +9164,41 @@
     </row>
     <row r="14" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="16" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
       </c>
       <c r="H14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="16" t="b">
-        <v>0</v>
+      <c r="I14" s="16">
+        <v>1</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
       <c r="P14" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
@@ -9204,43 +9207,43 @@
     </row>
     <row r="15" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="16" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
       </c>
       <c r="H15" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="16" t="b">
-        <v>0</v>
+      <c r="I15" s="16">
+        <v>1</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
@@ -9249,41 +9252,41 @@
     </row>
     <row r="16" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
       </c>
       <c r="H16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="16" t="b">
-        <v>0</v>
+      <c r="I16" s="16">
+        <v>1</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
       <c r="P16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
@@ -9292,41 +9295,41 @@
     </row>
     <row r="17" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1</v>
       </c>
       <c r="H17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="16" t="b">
-        <v>0</v>
+      <c r="I17" s="16">
+        <v>1</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
@@ -9358,23 +9361,23 @@
     </row>
     <row r="19" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="17" t="b">
-        <v>1</v>
+      <c r="I19" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
@@ -9383,51 +9386,51 @@
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="17" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0</v>
       </c>
       <c r="H20" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="17" t="b">
-        <v>0</v>
+      <c r="I20" s="17">
+        <v>1</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
@@ -9436,23 +9439,23 @@
     </row>
     <row r="21" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="17" t="b">
-        <v>1</v>
+      <c r="I21" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
@@ -9461,10 +9464,10 @@
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q21" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
@@ -9473,43 +9476,43 @@
     </row>
     <row r="22" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="17" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0</v>
       </c>
       <c r="H22" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="17" t="b">
-        <v>0</v>
+      <c r="I22" s="17">
+        <v>1</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q22" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
@@ -9535,43 +9538,43 @@
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
       </c>
       <c r="H24" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="16" t="b">
-        <v>0</v>
+      <c r="I24" s="16">
+        <v>1</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
@@ -9580,43 +9583,43 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="16" t="b">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
       </c>
       <c r="H25" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="16" t="b">
-        <v>0</v>
+      <c r="I25" s="16">
+        <v>1</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
       <c r="P25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
@@ -9625,80 +9628,80 @@
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
       </c>
       <c r="H26" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="16" t="b">
-        <v>0</v>
+      <c r="I26" s="16">
+        <v>1</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="16" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
       </c>
       <c r="H27" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="16" t="b">
-        <v>0</v>
+      <c r="I27" s="16">
+        <v>1</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q27" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
@@ -9730,41 +9733,41 @@
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="17" t="b">
+        <v>15</v>
+      </c>
+      <c r="G29" s="17">
         <v>0</v>
       </c>
       <c r="H29" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="17" t="b">
-        <v>0</v>
+      <c r="I29" s="17">
+        <v>1</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q29" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
@@ -9773,41 +9776,41 @@
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="17" t="b">
+        <v>15</v>
+      </c>
+      <c r="G30" s="17">
         <v>1</v>
       </c>
       <c r="H30" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="17" t="b">
-        <v>0</v>
+      <c r="I30" s="17">
+        <v>1</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
       <c r="L30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
@@ -9816,23 +9819,23 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="17" t="b">
-        <v>1</v>
+      <c r="I31" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
@@ -9841,10 +9844,10 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
@@ -9853,23 +9856,23 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="17" t="b">
-        <v>1</v>
+      <c r="I32" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
@@ -9878,10 +9881,10 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q32" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
@@ -9890,23 +9893,23 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="17" t="b">
-        <v>1</v>
+      <c r="I33" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
@@ -9915,10 +9918,10 @@
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
       <c r="P33" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
@@ -9927,84 +9930,84 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="17" t="b">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0</v>
       </c>
       <c r="H34" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="17" t="b">
-        <v>0</v>
+      <c r="I34" s="17">
+        <v>1</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N34" s="17"/>
       <c r="O34" s="17"/>
       <c r="P34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q34" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="17" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="G35" s="17">
+        <v>0</v>
       </c>
       <c r="H35" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="17" t="b">
-        <v>0</v>
+      <c r="I35" s="17">
+        <v>1</v>
       </c>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q35" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S35" s="8"/>
       <c r="T35" s="9"/>
@@ -10013,43 +10016,43 @@
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="17" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0</v>
       </c>
       <c r="H36" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="17" t="b">
-        <v>0</v>
+      <c r="I36" s="17">
+        <v>1</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N36" s="17"/>
       <c r="O36" s="17"/>
       <c r="P36" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S36" s="8"/>
       <c r="T36" s="9"/>
@@ -10058,41 +10061,41 @@
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1</v>
       </c>
       <c r="H37" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="17" t="b">
-        <v>0</v>
+      <c r="I37" s="17">
+        <v>1</v>
       </c>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
       <c r="P37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S37" s="8"/>
       <c r="T37" s="9"/>
@@ -10101,41 +10104,41 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G38" s="17">
+        <v>1</v>
       </c>
       <c r="H38" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="17" t="b">
-        <v>0</v>
+      <c r="I38" s="17">
+        <v>1</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S38" s="8"/>
       <c r="T38" s="9"/>
@@ -10164,23 +10167,23 @@
     </row>
     <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
-      <c r="I40" s="16" t="b">
-        <v>1</v>
+      <c r="I40" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
@@ -10189,51 +10192,51 @@
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q40" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="16" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G41" s="16">
+        <v>0</v>
       </c>
       <c r="H41" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="16" t="b">
-        <v>0</v>
+      <c r="I41" s="16">
+        <v>1</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
       <c r="P41" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10257,84 +10260,84 @@
     </row>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" s="17" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="G43" s="17">
+        <v>0</v>
       </c>
       <c r="H43" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="17" t="b">
-        <v>0</v>
+      <c r="I43" s="17">
+        <v>1</v>
       </c>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
       <c r="P43" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="17" t="b">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="G44" s="17">
+        <v>0</v>
       </c>
       <c r="H44" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="17" t="b">
-        <v>0</v>
+      <c r="I44" s="17">
+        <v>1</v>
       </c>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
       <c r="L44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N44" s="17"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10358,64 +10361,64 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="16" t="b">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="G46" s="16">
+        <v>0</v>
       </c>
       <c r="H46" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="16" t="b">
-        <v>0</v>
+      <c r="I46" s="16">
+        <v>1</v>
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
       <c r="L46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
       <c r="P46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="16" t="b">
-        <v>1</v>
+      <c r="I47" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>
@@ -10424,10 +10427,10 @@
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
       <c r="P47" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10451,64 +10454,64 @@
     </row>
     <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" s="17" t="b">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="G49" s="17">
+        <v>0</v>
       </c>
       <c r="H49" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="17" t="b">
-        <v>0</v>
+      <c r="I49" s="17">
+        <v>1</v>
       </c>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
-      <c r="I50" s="17" t="b">
-        <v>1</v>
+      <c r="I50" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -10517,49 +10520,49 @@
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
       <c r="P50" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q50" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
       <c r="F51" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="17" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G51" s="17">
+        <v>1</v>
       </c>
       <c r="H51" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="17" t="b">
-        <v>0</v>
+      <c r="I51" s="17">
+        <v>1</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q51" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10583,121 +10586,121 @@
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="16" t="b">
+        <v>15</v>
+      </c>
+      <c r="G53" s="16">
         <v>0</v>
       </c>
       <c r="H53" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="16" t="b">
-        <v>0</v>
+      <c r="I53" s="16">
+        <v>1</v>
       </c>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
       <c r="L53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
       <c r="P53" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q53" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G54" s="16" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="G54" s="16">
+        <v>0</v>
       </c>
       <c r="H54" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="16" t="b">
-        <v>0</v>
+      <c r="I54" s="16">
+        <v>1</v>
       </c>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
       <c r="L54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
       <c r="P54" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q54" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="16" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G55" s="16">
+        <v>1</v>
       </c>
       <c r="H55" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I55" s="16" t="b">
-        <v>0</v>
+      <c r="I55" s="16">
+        <v>1</v>
       </c>
       <c r="J55" s="16"/>
       <c r="K55" s="16"/>
       <c r="L55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N55" s="16"/>
       <c r="O55" s="16"/>
       <c r="P55" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q55" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10721,41 +10724,41 @@
     </row>
     <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="17" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G57" s="17">
+        <v>1</v>
       </c>
       <c r="H57" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="17" t="b">
-        <v>0</v>
+      <c r="I57" s="17">
+        <v>1</v>
       </c>
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
       <c r="L57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N57" s="17"/>
       <c r="O57" s="17"/>
       <c r="P57" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q57" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10779,80 +10782,80 @@
     </row>
     <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="F59" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G59" s="16">
+        <v>1</v>
       </c>
       <c r="H59" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I59" s="16" t="b">
-        <v>0</v>
+      <c r="I59" s="16">
+        <v>1</v>
       </c>
       <c r="J59" s="16"/>
       <c r="K59" s="16"/>
       <c r="L59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
       <c r="P59" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q59" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" s="16" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G60" s="16">
+        <v>1</v>
       </c>
       <c r="H60" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I60" s="16" t="b">
-        <v>0</v>
+      <c r="I60" s="16">
+        <v>1</v>
       </c>
       <c r="J60" s="16"/>
       <c r="K60" s="16"/>
       <c r="L60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N60" s="16"/>
       <c r="O60" s="16"/>
       <c r="P60" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10876,23 +10879,23 @@
     </row>
     <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
-      <c r="I62" s="17" t="b">
-        <v>1</v>
+      <c r="I62" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
@@ -10901,10 +10904,10 @@
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
       <c r="P62" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q62" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10928,23 +10931,23 @@
     </row>
     <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
       <c r="E64" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="16" t="b">
-        <v>1</v>
+      <c r="I64" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
@@ -10953,10 +10956,10 @@
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
       <c r="P64" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q64" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10980,41 +10983,41 @@
     </row>
     <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" s="17" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G66" s="17">
+        <v>0</v>
       </c>
       <c r="H66" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I66" s="17" t="b">
-        <v>0</v>
+      <c r="I66" s="17">
+        <v>1</v>
       </c>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
       <c r="L66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="M66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="M66" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="N66" s="17"/>
       <c r="O66" s="17"/>
       <c r="P66" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q66" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="Q66" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11038,84 +11041,84 @@
     </row>
     <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G68" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G68" s="16">
+        <v>0</v>
       </c>
       <c r="H68" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I68" s="16" t="b">
-        <v>0</v>
+      <c r="I68" s="16">
+        <v>1</v>
       </c>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
       <c r="L68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="M68" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
       <c r="P68" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q68" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="Q68" s="16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G69" s="16" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="G69" s="16">
+        <v>0</v>
       </c>
       <c r="H69" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I69" s="16" t="b">
-        <v>0</v>
+      <c r="I69" s="16">
+        <v>1</v>
       </c>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
       <c r="L69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
       <c r="P69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q69" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11139,41 +11142,41 @@
     </row>
     <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G71" s="17" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G71" s="17">
+        <v>1</v>
       </c>
       <c r="H71" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I71" s="17" t="b">
-        <v>0</v>
+      <c r="I71" s="17">
+        <v>1</v>
       </c>
       <c r="J71" s="17"/>
       <c r="K71" s="17"/>
       <c r="L71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="M71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="M71" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="N71" s="17"/>
       <c r="O71" s="17"/>
       <c r="P71" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q71" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="Q71" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11197,41 +11200,41 @@
     </row>
     <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="16" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G73" s="16">
+        <v>0</v>
       </c>
       <c r="H73" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="I73" s="16" t="b">
-        <v>0</v>
+      <c r="I73" s="16">
+        <v>1</v>
       </c>
       <c r="J73" s="16"/>
       <c r="K73" s="16"/>
       <c r="L73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N73" s="16"/>
       <c r="O73" s="16"/>
       <c r="P73" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q73" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11255,41 +11258,41 @@
     </row>
     <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G75" s="17" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G75" s="17">
+        <v>0</v>
       </c>
       <c r="H75" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="17" t="b">
-        <v>0</v>
+      <c r="I75" s="17">
+        <v>1</v>
       </c>
       <c r="J75" s="17"/>
       <c r="K75" s="17"/>
       <c r="L75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N75" s="17"/>
       <c r="O75" s="17"/>
       <c r="P75" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q75" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -24415,7 +24418,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -24444,369 +24447,369 @@
     </row>
     <row r="2" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -25806,7 +25809,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -25834,190 +25837,190 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
replace container with require
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F363B6-F73D-794F-9068-3A4672994DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC4E2C-590D-8E43-A76C-552FA949B5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,16 +387,16 @@
     <t>btree:name(cursorable=False)</t>
   </si>
   <si>
-    <t>requires:power_EnergyArea(container=EnergyArea)</t>
+    <t>requires:power_GeneratingUnit(require=GeneratingUnit)</t>
   </si>
   <si>
-    <t>requires:power_Substation(container=Substation)</t>
+    <t>requires:power_EnergyArea(require=EnergyArea)</t>
   </si>
   <si>
-    <t>requires:power_GeoLocation(container=GeoLocation)</t>
+    <t>requires:power_Substation(require=Substation)</t>
   </si>
   <si>
-    <t>requires:power_GeneratingUnit(container=GeneratingUnit)</t>
+    <t>requires:power_GeoLocation(require=GeoLocation)</t>
   </si>
 </sst>
 </file>
@@ -25809,7 +25809,7 @@
   <dimension ref="A1:X1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25884,7 +25884,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -25905,7 +25905,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -25926,7 +25926,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
@@ -25941,7 +25941,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
@@ -25993,7 +25993,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Replace container with require  (#1339)
# Description

This PR proactively fixes issue with compatibility of v0 and v1 of neat

## Bump

- [ ] Patch
- [X] Minor
- [ ] Skip

## Changelog
### Changed

- Requires constraint are now set by stating container via property
`require` , which was previously `container`
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
+++ b/docs/artifacts/rules/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F363B6-F73D-794F-9068-3A4672994DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC4E2C-590D-8E43-A76C-552FA949B5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,16 +387,16 @@
     <t>btree:name(cursorable=False)</t>
   </si>
   <si>
-    <t>requires:power_EnergyArea(container=EnergyArea)</t>
+    <t>requires:power_GeneratingUnit(require=GeneratingUnit)</t>
   </si>
   <si>
-    <t>requires:power_Substation(container=Substation)</t>
+    <t>requires:power_EnergyArea(require=EnergyArea)</t>
   </si>
   <si>
-    <t>requires:power_GeoLocation(container=GeoLocation)</t>
+    <t>requires:power_Substation(require=Substation)</t>
   </si>
   <si>
-    <t>requires:power_GeneratingUnit(container=GeneratingUnit)</t>
+    <t>requires:power_GeoLocation(require=GeoLocation)</t>
   </si>
 </sst>
 </file>
@@ -25809,7 +25809,7 @@
   <dimension ref="A1:X1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25884,7 +25884,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -25905,7 +25905,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -25926,7 +25926,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
@@ -25941,7 +25941,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
@@ -25993,7 +25993,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>

</xml_diff>